<commit_message>
Add support for tabs to 3d model page, support axis customization
</commit_message>
<xml_diff>
--- a/config_portal/examples/obj-files.xlsx
+++ b/config_portal/examples/obj-files.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlabyer/Projects/tde-test/tissue-data-explorer/config_portal/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlabyer/Projects/tissue-data-explorer/config_portal/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190894AD-5170-034C-B555-61BFDB4E3FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3BA79F-3493-5C4C-98B6-3EC1CE3A82F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="1300" windowWidth="27640" windowHeight="16940" xr2:uid="{3D5C0E23-C149-624D-A4EA-1CF568E3B69C}"/>
   </bookViews>
   <sheets>
     <sheet name="files" sheetId="1" r:id="rId1"/>
+    <sheet name="notes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
   <si>
     <t>Body</t>
   </si>
@@ -114,18 +115,51 @@
   </si>
   <si>
     <t>S1_Sphere_Upper_S1-15.obj</t>
+  </si>
+  <si>
+    <t>x axis</t>
+  </si>
+  <si>
+    <t>y axis</t>
+  </si>
+  <si>
+    <t>z axis</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>Plotly Dash Coordinate Axes</t>
+  </si>
+  <si>
+    <t>The Plotly Dash 3d surface capability displays data using a right-handed coordinate system with the z axis extending in the vertical direction. 
+If you want to display your data differently, you can map the axes in your data to Plotly's axes using the vector columns in the files tab. This will cause the data to be labelled according to Plotly's axes labelling. So if you map your z axis to Plotly's y axis, it will be labelled as the y axis in the resulting plot.
+Valid mapping values are x, y, and z.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -149,8 +183,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A2B076-C05F-964F-BD37-33F7D597451D}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,7 +535,7 @@
     <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -513,8 +551,17 @@
       <c r="E1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -530,8 +577,17 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -547,8 +603,17 @@
       <c r="E3">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -564,8 +629,17 @@
       <c r="E4">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -581,8 +655,17 @@
       <c r="E5">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -598,8 +681,17 @@
       <c r="E6">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -615,8 +707,17 @@
       <c r="E7">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -632,8 +733,17 @@
       <c r="E8">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -649,8 +759,17 @@
       <c r="E9">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -665,6 +784,43 @@
       </c>
       <c r="E10">
         <v>0.6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E3002E-10AA-BF43-B973-3F5A526C5CB5}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="63.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="153" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>